<commit_message>
Resolve bug that automation could not match education keyword, removed testing log messages
</commit_message>
<xml_diff>
--- a/KeywordLibrary.xlsx
+++ b/KeywordLibrary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\Personal\UiPath\RPA-J-01 Job matching for Placements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3F6B4E-0B7E-42F7-AA7A-38BBA3B27605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A543240-CDBD-4C66-90FC-EDB1603D5054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3375" windowWidth="29430" windowHeight="15345" xr2:uid="{4FC0F06C-D9D6-45DE-B83F-4A922B31FC97}"/>
+    <workbookView xWindow="1065" yWindow="3090" windowWidth="32280" windowHeight="15345" activeTab="1" xr2:uid="{4FC0F06C-D9D6-45DE-B83F-4A922B31FC97}"/>
   </bookViews>
   <sheets>
     <sheet name="keyword CV" sheetId="1" r:id="rId1"/>
@@ -1594,10 +1594,10 @@
     <t>Job Search Keyword</t>
   </si>
   <si>
-    <t>rpa</t>
-  </si>
-  <si>
     <t>bachelor</t>
+  </si>
+  <si>
+    <t>rpa developer</t>
   </si>
 </sst>
 </file>
@@ -1963,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCB9B35-F431-45F4-8A59-C98B611EF534}">
   <dimension ref="A1:B501"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -2015,7 +2015,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>27</v>
@@ -4557,8 +4557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AB57A9-B4A8-4B96-8BE3-DC53E93A2380}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4573,7 +4573,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>

</xml_diff>